<commit_message>
análise preliminar - ajuste n-shot
</commit_message>
<xml_diff>
--- a/data/Analise.xlsx
+++ b/data/Analise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo\source\repos\exqa-complearning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E3C186-9EE9-4AEB-9EA3-C18990A910AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8380DC8A-5D89-487A-86B2-2A636D42EE2B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{26B1A209-A022-4AEA-B0B7-51D88A9CAA44}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="115">
   <si>
     <t>cod</t>
   </si>
@@ -369,6 +369,21 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Shots</t>
+  </si>
+  <si>
+    <t>2-shot</t>
+  </si>
+  <si>
+    <t>3-shot</t>
+  </si>
+  <si>
+    <t>1-shot</t>
+  </si>
+  <si>
+    <t>0-shot</t>
   </si>
 </sst>
 </file>
@@ -377,7 +392,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -507,20 +522,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,227 +543,6 @@
     <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="17">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -824,6 +618,227 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color theme="4"/>
+        </bottom>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1507,16 +1522,16 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Desempenho médio'!$B$21:$D$21</c:f>
+              <c:f>'Desempenho médio'!$B$21:$E$21</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>transfer</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>en</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>distilbert-base-cased-distilled-squad</c:v>
                 </c:pt>
               </c:strCache>
@@ -1548,17 +1563,17 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Desempenho médio'!$E$20:$H$20</c:f>
+              <c:f>'Desempenho médio'!$F$20:$I$20</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>EM</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>EM@3</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>F1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>EM@3</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>F1@3</c:v>
@@ -1568,21 +1583,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Desempenho médio'!$E$21:$H$21</c:f>
+              <c:f>'Desempenho médio'!$F$21:$I$21</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.7833</c:v>
+                  <c:v>0.72199999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.85930000000000006</c:v>
+                  <c:v>0.84549999999999992</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.87930000000000008</c:v>
+                  <c:v>0.83169999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.91909999999999992</c:v>
+                  <c:v>0.89739999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1599,16 +1614,16 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Desempenho médio'!$B$22:$D$22</c:f>
+              <c:f>'Desempenho médio'!$B$22:$E$22</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>transfer</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>pt</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>pierreguillou/bert-large-cased-squad-v1.1-portuguese</c:v>
                 </c:pt>
               </c:strCache>
@@ -1640,17 +1655,17 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Desempenho médio'!$E$20:$H$20</c:f>
+              <c:f>'Desempenho médio'!$F$20:$I$20</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>EM</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>EM@3</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>F1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>EM@3</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>F1@3</c:v>
@@ -1660,21 +1675,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Desempenho médio'!$E$22:$H$22</c:f>
+              <c:f>'Desempenho médio'!$F$22:$I$22</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.72170000000000001</c:v>
+                  <c:v>0.72140000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.83134999999999992</c:v>
+                  <c:v>0.84409999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.84479999999999988</c:v>
+                  <c:v>0.83099999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.89694999999999991</c:v>
+                  <c:v>0.89650000000000007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1691,16 +1706,19 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Desempenho médio'!$B$23:$D$23</c:f>
+              <c:f>'Desempenho médio'!$B$23:$E$23</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>context</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>2-shot</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>en</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>EleutherAI/gpt-neo-2.7B</c:v>
                 </c:pt>
               </c:strCache>
@@ -1732,17 +1750,17 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Desempenho médio'!$E$20:$H$20</c:f>
+              <c:f>'Desempenho médio'!$F$20:$I$20</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>EM</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>EM@3</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>F1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>EM@3</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>F1@3</c:v>
@@ -1752,21 +1770,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Desempenho médio'!$E$23:$H$23</c:f>
+              <c:f>'Desempenho médio'!$F$23:$I$23</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.38019999999999998</c:v>
+                  <c:v>0.46189999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.50905</c:v>
+                  <c:v>0.53700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.43965000000000004</c:v>
+                  <c:v>0.58520000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.59184999999999999</c:v>
+                  <c:v>0.68330000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1783,17 +1801,20 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Desempenho médio'!$B$24:$D$24</c:f>
+              <c:f>'Desempenho médio'!$B$24:$E$24</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>context</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>3-shot</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>en</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>EleutherAI/gpt-neo-1.3B</c:v>
+                <c:pt idx="3">
+                  <c:v>EleutherAI/gpt-neo-2.7B</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1824,17 +1845,17 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Desempenho médio'!$E$20:$H$20</c:f>
+              <c:f>'Desempenho médio'!$F$20:$I$20</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>EM</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>EM@3</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>F1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>EM@3</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>F1@3</c:v>
@@ -1844,21 +1865,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Desempenho médio'!$E$24:$H$24</c:f>
+              <c:f>'Desempenho médio'!$F$24:$I$24</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.31162499999999999</c:v>
+                  <c:v>0.45069999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.44155</c:v>
+                  <c:v>0.50819999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.3639750000000001</c:v>
+                  <c:v>0.58789999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.51910000000000001</c:v>
+                  <c:v>0.66849999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1875,17 +1896,20 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Desempenho médio'!$B$25:$D$25</c:f>
+              <c:f>'Desempenho médio'!$B$25:$E$25</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>context</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>1-shot</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>en</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>EleutherAI/gpt-j-6B</c:v>
+                <c:pt idx="3">
+                  <c:v>EleutherAI/gpt-neo-2.7B</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1916,17 +1940,17 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Desempenho médio'!$E$20:$H$20</c:f>
+              <c:f>'Desempenho médio'!$F$20:$I$20</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>EM</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>EM@3</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>F1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>EM@3</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>F1@3</c:v>
@@ -1936,21 +1960,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Desempenho médio'!$E$25:$H$25</c:f>
+              <c:f>'Desempenho médio'!$F$25:$I$25</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.30959999999999999</c:v>
+                  <c:v>0.4385</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.39490000000000003</c:v>
+                  <c:v>0.51249999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.36380000000000001</c:v>
+                  <c:v>0.56930000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.47889999999999999</c:v>
+                  <c:v>0.66310000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1959,6 +1983,606 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-6FCB-4673-930F-6AC163E2225A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Desempenho médio'!$B$26:$E$26</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>context</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2-shot</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>en</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EleutherAI/gpt-neo-1.3B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Desempenho médio'!$F$20:$I$20</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>EM</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>EM@3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>F1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>F1@3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Desempenho médio'!$F$26:$I$26</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.38719999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4572</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.51419999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.60680000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5119-4ED4-BEC3-6BBD19ECC0EC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Desempenho médio'!$B$27:$E$27</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>context</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1-shot</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>en</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EleutherAI/gpt-neo-1.3B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Desempenho médio'!$F$20:$I$20</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>EM</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>EM@3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>F1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>F1@3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Desempenho médio'!$F$27:$I$27</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.3614</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.42770000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.57940000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5119-4ED4-BEC3-6BBD19ECC0EC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Desempenho médio'!$B$28:$E$28</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>context</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3-shot</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>en</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EleutherAI/gpt-neo-1.3B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Desempenho médio'!$F$20:$I$20</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>EM</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>EM@3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>F1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>F1@3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Desempenho médio'!$F$28:$I$28</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.35369999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.40429999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.49020000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.56689999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-5119-4ED4-BEC3-6BBD19ECC0EC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Desempenho médio'!$B$29:$E$29</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>context</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0-shot</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>en</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EleutherAI/gpt-j-6B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Desempenho médio'!$F$20:$I$20</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>EM</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>EM@3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>F1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>F1@3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Desempenho médio'!$F$29:$I$29</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.30959999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.36380000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.39490000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.47889999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-5119-4ED4-BEC3-6BBD19ECC0EC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Desempenho médio'!$B$30:$E$30</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>context</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0-shot</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>en</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EleutherAI/gpt-neo-2.7B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Desempenho médio'!$F$20:$I$20</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>EM</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>EM@3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>F1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>F1@3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Desempenho médio'!$F$30:$I$30</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.16969999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2009</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.29380000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.35249999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-5119-4ED4-BEC3-6BBD19ECC0EC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Desempenho médio'!$B$31:$E$31</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>context</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0-shot</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>en</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>EleutherAI/gpt-neo-1.3B</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Desempenho médio'!$F$20:$I$20</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>EM</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>EM@3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>F1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>F1@3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Desempenho médio'!$F$31:$I$31</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.14419999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.16670000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.27379999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.32329999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-5119-4ED4-BEC3-6BBD19ECC0EC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3872,15 +4496,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>45720</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>3810</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>274320</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>83820</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3910,10 +4534,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{714E93ED-62C2-48B4-8258-BDFBEDF15324}" name="Tabela2" displayName="Tabela2" ref="A19:B24" totalsRowShown="0" headerRowBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{714E93ED-62C2-48B4-8258-BDFBEDF15324}" name="Tabela2" displayName="Tabela2" ref="A19:B24" totalsRowShown="0" headerRowBorderDxfId="16">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{C7E5CCC0-2C70-4E0C-B797-1F9D4950D468}" name="Modelo avaliado" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{CDC66701-1873-4136-8779-43DB08CD082C}" name="Duração por questão (ms)" dataDxfId="0" dataCellStyle="Vírgula">
+    <tableColumn id="1" xr3:uid="{C7E5CCC0-2C70-4E0C-B797-1F9D4950D468}" name="Modelo avaliado" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{CDC66701-1873-4136-8779-43DB08CD082C}" name="Duração por questão (ms)" dataDxfId="14" dataCellStyle="Vírgula">
       <calculatedColumnFormula>SUMIF(duração!$D$2:$D$50,$A2,duração!F$2:F$50)/COUNTIF(duração!$D$2:$D$50,$A2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3922,10 +4546,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{35C1D468-735A-4719-B6AA-CE990286634A}" name="Tabela3" displayName="Tabela3" ref="A1:B6" totalsRowShown="0" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{35C1D468-735A-4719-B6AA-CE990286634A}" name="Tabela3" displayName="Tabela3" ref="A1:B6" totalsRowShown="0" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{1FB3AE1F-72BC-455D-B745-25296ABF8784}" name="Modelo avaliado" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{CA4FEEBD-B236-4446-AAE4-8A47525ECB6B}" name="Duração Total (s)" dataDxfId="7" dataCellStyle="Vírgula">
+    <tableColumn id="1" xr3:uid="{1FB3AE1F-72BC-455D-B745-25296ABF8784}" name="Modelo avaliado" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{CA4FEEBD-B236-4446-AAE4-8A47525ECB6B}" name="Duração Total (s)" dataDxfId="9" dataCellStyle="Vírgula">
       <calculatedColumnFormula>SUMIF(duração!$D$2:$D$50,$A2,duração!E$2:E$50)/COUNTIF(duração!$D$2:$D$50,$A2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3934,22 +4558,23 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CCB9E723-84F3-4D8B-A97F-0B55F263F060}" name="Tabela1" displayName="Tabela1" ref="B20:H25" totalsRowShown="0" dataDxfId="12" dataCellStyle="Porcentagem">
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CCB9E723-84F3-4D8B-A97F-0B55F263F060}" name="Tabela1" displayName="Tabela1" ref="B20:I31" totalsRowShown="0" dataDxfId="8" dataCellStyle="Porcentagem">
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{93ADF30E-F57C-49C0-B5E8-C5488A6A83F0}" name="Tipo"/>
+    <tableColumn id="8" xr3:uid="{CE0ED6A0-317E-457B-BF71-6FC9675AC4EE}" name="Shots"/>
     <tableColumn id="2" xr3:uid="{FF67D44E-6ED4-4F89-AF15-CC8EBE3465E3}" name="Linguagem"/>
     <tableColumn id="3" xr3:uid="{1DC30509-F188-4F99-8A44-BDBEF19B0ABA}" name="Modelo avaliado"/>
-    <tableColumn id="4" xr3:uid="{E1D10458-1127-45BD-969F-BA3FBEC55DF3}" name="EM" dataDxfId="16" dataCellStyle="Porcentagem">
-      <calculatedColumnFormula>SUMIF($D$2:$D$14,$D21,E$2:E$14)/COUNTIF($D$2:$D$14,$D21)/100</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{E1D10458-1127-45BD-969F-BA3FBEC55DF3}" name="EM" dataDxfId="3" dataCellStyle="Porcentagem">
+      <calculatedColumnFormula>F4/100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B6E2BB96-BE19-4C5D-A95E-A1A468D55E24}" name="F1" dataDxfId="15" dataCellStyle="Porcentagem">
-      <calculatedColumnFormula>SUMIF($D$2:$D$14,$D21,F$2:F$14)/COUNTIF($D$2:$D$14,$D21)/100</calculatedColumnFormula>
+    <tableColumn id="5" xr3:uid="{B6E2BB96-BE19-4C5D-A95E-A1A468D55E24}" name="EM@3" dataDxfId="1" dataCellStyle="Porcentagem">
+      <calculatedColumnFormula>G4/100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{2D068FAA-A80A-440E-9829-CB6CCADED338}" name="EM@3" dataDxfId="14" dataCellStyle="Porcentagem">
-      <calculatedColumnFormula>SUMIF($D$2:$D$14,$D21,G$2:G$14)/COUNTIF($D$2:$D$14,$D21)/100</calculatedColumnFormula>
+    <tableColumn id="6" xr3:uid="{2D068FAA-A80A-440E-9829-CB6CCADED338}" name="F1" dataDxfId="0" dataCellStyle="Porcentagem">
+      <calculatedColumnFormula>H4/100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{2EAB6646-3388-4DF1-A9B9-03C3EA61FCDC}" name="F1@3" dataDxfId="13" dataCellStyle="Porcentagem">
-      <calculatedColumnFormula>SUMIF($D$2:$D$14,$D21,H$2:H$14)/COUNTIF($D$2:$D$14,$D21)/100</calculatedColumnFormula>
+    <tableColumn id="7" xr3:uid="{2EAB6646-3388-4DF1-A9B9-03C3EA61FCDC}" name="F1@3" dataDxfId="2" dataCellStyle="Porcentagem">
+      <calculatedColumnFormula>I4/100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3957,20 +4582,20 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{97E42113-0461-4359-82B5-3B8C78349CE7}" name="Tabela4" displayName="Tabela4" ref="D29:H30" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{97E42113-0461-4359-82B5-3B8C78349CE7}" name="Tabela4" displayName="Tabela4" ref="E36:I37" totalsRowShown="0">
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{3F65CCCC-D216-4E94-AC61-60DC20E780EB}" name=" "/>
-    <tableColumn id="2" xr3:uid="{56C7062A-4FB0-49AF-96F0-06C76D3FB6CF}" name="EM" dataDxfId="6">
-      <calculatedColumnFormula>E21-E23</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{31BF2B87-4552-469C-AB09-5BDA978CF82F}" name="F1" dataDxfId="5">
+    <tableColumn id="2" xr3:uid="{56C7062A-4FB0-49AF-96F0-06C76D3FB6CF}" name="EM" dataDxfId="7">
       <calculatedColumnFormula>F21-F23</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{16935C24-6567-401E-8B85-3737EE40B64D}" name="EM@3" dataDxfId="4">
+    <tableColumn id="3" xr3:uid="{31BF2B87-4552-469C-AB09-5BDA978CF82F}" name="EM@3" dataDxfId="6">
       <calculatedColumnFormula>G21-G23</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{2D45CC25-E94A-4498-873A-B2E9E96EFDD2}" name="F1@3" dataDxfId="3">
+    <tableColumn id="4" xr3:uid="{16935C24-6567-401E-8B85-3737EE40B64D}" name="F1" dataDxfId="5">
       <calculatedColumnFormula>H21-H23</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{2D45CC25-E94A-4498-873A-B2E9E96EFDD2}" name="F1@3" dataDxfId="4">
+      <calculatedColumnFormula>I21-I23</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4277,7 +4902,7 @@
   <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="C3" sqref="C3:N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7529,19 +8154,19 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA034621-946B-45D7-A78A-94802C0DA0D4}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29:H30"/>
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.5546875" customWidth="1"/>
-    <col min="4" max="4" width="45.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="5" max="5" width="45.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>102</v>
       </c>
@@ -7549,561 +8174,783 @@
         <v>99</v>
       </c>
       <c r="C1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" t="s">
         <v>101</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>100</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>43</v>
-      </c>
-      <c r="F1" t="s">
-        <v>45</v>
       </c>
       <c r="G1" t="s">
         <v>47</v>
       </c>
       <c r="H1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>28</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="4">
+      <c r="F2" s="4">
         <v>78.34</v>
-      </c>
-      <c r="F2" s="4">
-        <v>85.94</v>
       </c>
       <c r="G2" s="4">
         <v>88</v>
       </c>
       <c r="H2" s="4">
+        <v>85.94</v>
+      </c>
+      <c r="I2" s="4">
         <v>91.98</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>28</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="4">
+      <c r="F3" s="4">
         <v>78.319999999999993</v>
-      </c>
-      <c r="F3" s="4">
-        <v>85.92</v>
       </c>
       <c r="G3" s="4">
         <v>87.86</v>
       </c>
       <c r="H3" s="4">
+        <v>85.92</v>
+      </c>
+      <c r="I3" s="4">
         <v>91.84</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="4">
+      <c r="F4" s="4">
         <v>72.2</v>
-      </c>
-      <c r="F4" s="4">
-        <v>83.17</v>
       </c>
       <c r="G4" s="4">
         <v>84.55</v>
       </c>
       <c r="H4" s="4">
+        <v>83.17</v>
+      </c>
+      <c r="I4" s="4">
         <v>89.74</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>16</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>21</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="4">
+      <c r="F5" s="4">
         <v>72.14</v>
-      </c>
-      <c r="F5" s="4">
-        <v>83.1</v>
       </c>
       <c r="G5" s="4">
         <v>84.41</v>
       </c>
       <c r="H5" s="4">
+        <v>83.1</v>
+      </c>
+      <c r="I5" s="4">
         <v>89.65</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>25</v>
       </c>
       <c r="B6" t="s">
         <v>30</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
         <v>28</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="4">
+      <c r="F6" s="4">
         <v>46.19</v>
-      </c>
-      <c r="F6" s="4">
-        <v>58.52</v>
       </c>
       <c r="G6" s="4">
         <v>53.7</v>
       </c>
       <c r="H6" s="4">
+        <v>58.52</v>
+      </c>
+      <c r="I6" s="4">
         <v>68.33</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>26</v>
       </c>
       <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
         <v>28</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="4">
+      <c r="F7" s="4">
         <v>45.07</v>
-      </c>
-      <c r="F7" s="4">
-        <v>58.79</v>
       </c>
       <c r="G7" s="4">
         <v>50.82</v>
       </c>
       <c r="H7" s="4">
+        <v>58.79</v>
+      </c>
+      <c r="I7" s="4">
         <v>66.849999999999994</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>24</v>
       </c>
       <c r="B8" t="s">
         <v>30</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
         <v>28</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="4">
+      <c r="F8" s="4">
         <v>43.85</v>
-      </c>
-      <c r="F8" s="4">
-        <v>56.93</v>
       </c>
       <c r="G8" s="4">
         <v>51.25</v>
       </c>
       <c r="H8" s="4">
+        <v>56.93</v>
+      </c>
+      <c r="I8" s="4">
         <v>66.31</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>21</v>
       </c>
       <c r="B9" t="s">
         <v>30</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
         <v>28</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="4">
+      <c r="F9" s="4">
         <v>38.72</v>
-      </c>
-      <c r="F9" s="4">
-        <v>51.42</v>
       </c>
       <c r="G9" s="4">
         <v>45.72</v>
       </c>
       <c r="H9" s="4">
+        <v>51.42</v>
+      </c>
+      <c r="I9" s="4">
         <v>60.68</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>20</v>
       </c>
       <c r="B10" t="s">
         <v>30</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
         <v>28</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="4">
+      <c r="F10" s="4">
         <v>36.14</v>
-      </c>
-      <c r="F10" s="4">
-        <v>48.8</v>
       </c>
       <c r="G10" s="4">
         <v>42.77</v>
       </c>
       <c r="H10" s="4">
+        <v>48.8</v>
+      </c>
+      <c r="I10" s="4">
         <v>57.94</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>22</v>
       </c>
       <c r="B11" t="s">
         <v>30</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
         <v>28</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="4">
+      <c r="F11" s="4">
         <v>35.369999999999997</v>
-      </c>
-      <c r="F11" s="4">
-        <v>49.02</v>
       </c>
       <c r="G11" s="4">
         <v>40.43</v>
       </c>
       <c r="H11" s="4">
+        <v>49.02</v>
+      </c>
+      <c r="I11" s="4">
         <v>56.69</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>18</v>
       </c>
       <c r="B12" t="s">
         <v>30</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
         <v>28</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="4">
+      <c r="F12" s="4">
         <v>30.96</v>
-      </c>
-      <c r="F12" s="4">
-        <v>39.49</v>
       </c>
       <c r="G12" s="4">
         <v>36.380000000000003</v>
       </c>
       <c r="H12" s="4">
+        <v>39.49</v>
+      </c>
+      <c r="I12" s="4">
         <v>47.89</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>23</v>
       </c>
       <c r="B13" t="s">
         <v>30</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
         <v>28</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="4">
+      <c r="F13" s="4">
         <v>16.97</v>
-      </c>
-      <c r="F13" s="4">
-        <v>29.38</v>
       </c>
       <c r="G13" s="4">
         <v>20.09</v>
       </c>
       <c r="H13" s="4">
+        <v>29.38</v>
+      </c>
+      <c r="I13" s="4">
         <v>35.25</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>19</v>
       </c>
       <c r="B14" t="s">
         <v>30</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
         <v>28</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="4">
+      <c r="F14" s="4">
         <v>14.42</v>
-      </c>
-      <c r="F14" s="4">
-        <v>27.38</v>
       </c>
       <c r="G14" s="4">
         <v>16.670000000000002</v>
       </c>
       <c r="H14" s="4">
+        <v>27.38</v>
+      </c>
+      <c r="I14" s="4">
         <v>32.33</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>108</v>
       </c>
       <c r="C20" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20" t="s">
         <v>101</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>100</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>43</v>
-      </c>
-      <c r="F20" t="s">
-        <v>45</v>
       </c>
       <c r="G20" t="s">
         <v>47</v>
       </c>
       <c r="H20" t="s">
+        <v>45</v>
+      </c>
+      <c r="I20" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>20</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>28</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="5">
-        <f>SUMIF($D$2:$D$14,$D21,E$2:E$14)/COUNTIF($D$2:$D$14,$D21)/100</f>
-        <v>0.7833</v>
-      </c>
       <c r="F21" s="5">
-        <f t="shared" ref="F21:H21" si="0">SUMIF($D$2:$D$14,$D21,F$2:F$14)/COUNTIF($D$2:$D$14,$D21)/100</f>
-        <v>0.85930000000000006</v>
+        <f t="shared" ref="F21:F31" si="0">F4/100</f>
+        <v>0.72199999999999998</v>
       </c>
       <c r="G21" s="5">
-        <f t="shared" si="0"/>
-        <v>0.87930000000000008</v>
+        <f t="shared" ref="G21:G31" si="1">G4/100</f>
+        <v>0.84549999999999992</v>
       </c>
       <c r="H21" s="5">
-        <f t="shared" si="0"/>
-        <v>0.91909999999999992</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+        <f t="shared" ref="H21:H31" si="2">H4/100</f>
+        <v>0.83169999999999999</v>
+      </c>
+      <c r="I21" s="5">
+        <f t="shared" ref="I21:I31" si="3">I4/100</f>
+        <v>0.89739999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>20</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>21</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="5">
-        <f t="shared" ref="E22:H25" si="1">SUMIF($D$2:$D$14,$D22,E$2:E$14)/COUNTIF($D$2:$D$14,$D22)/100</f>
-        <v>0.72170000000000001</v>
-      </c>
       <c r="F22" s="5">
-        <f t="shared" si="1"/>
-        <v>0.83134999999999992</v>
+        <f t="shared" si="0"/>
+        <v>0.72140000000000004</v>
       </c>
       <c r="G22" s="5">
         <f t="shared" si="1"/>
-        <v>0.84479999999999988</v>
+        <v>0.84409999999999996</v>
       </c>
       <c r="H22" s="5">
-        <f t="shared" si="1"/>
-        <v>0.89694999999999991</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="I22" s="5">
+        <f t="shared" si="3"/>
+        <v>0.89650000000000007</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>30</v>
       </c>
       <c r="C23" t="s">
+        <v>111</v>
+      </c>
+      <c r="D23" t="s">
         <v>28</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>39</v>
       </c>
-      <c r="E23" s="5">
-        <f t="shared" si="1"/>
-        <v>0.38019999999999998</v>
-      </c>
       <c r="F23" s="5">
-        <f t="shared" si="1"/>
-        <v>0.50905</v>
+        <f t="shared" si="0"/>
+        <v>0.46189999999999998</v>
       </c>
       <c r="G23" s="5">
         <f t="shared" si="1"/>
-        <v>0.43965000000000004</v>
+        <v>0.53700000000000003</v>
       </c>
       <c r="H23" s="5">
-        <f t="shared" si="1"/>
-        <v>0.59184999999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0.58520000000000005</v>
+      </c>
+      <c r="I23" s="5">
+        <f t="shared" si="3"/>
+        <v>0.68330000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>30</v>
       </c>
       <c r="C24" t="s">
+        <v>112</v>
+      </c>
+      <c r="D24" t="s">
         <v>28</v>
       </c>
-      <c r="D24" t="s">
-        <v>35</v>
-      </c>
-      <c r="E24" s="5">
-        <f t="shared" si="1"/>
-        <v>0.31162499999999999</v>
+      <c r="E24" t="s">
+        <v>39</v>
       </c>
       <c r="F24" s="5">
-        <f t="shared" si="1"/>
-        <v>0.44155</v>
+        <f t="shared" si="0"/>
+        <v>0.45069999999999999</v>
       </c>
       <c r="G24" s="5">
         <f t="shared" si="1"/>
-        <v>0.3639750000000001</v>
+        <v>0.50819999999999999</v>
       </c>
       <c r="H24" s="5">
-        <f t="shared" si="1"/>
-        <v>0.51910000000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>0.58789999999999998</v>
+      </c>
+      <c r="I24" s="5">
+        <f t="shared" si="3"/>
+        <v>0.66849999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>30</v>
       </c>
       <c r="C25" t="s">
+        <v>113</v>
+      </c>
+      <c r="D25" t="s">
         <v>28</v>
       </c>
-      <c r="D25" t="s">
-        <v>31</v>
-      </c>
-      <c r="E25" s="5">
-        <f t="shared" si="1"/>
-        <v>0.30959999999999999</v>
+      <c r="E25" t="s">
+        <v>39</v>
       </c>
       <c r="F25" s="5">
-        <f t="shared" si="1"/>
-        <v>0.39490000000000003</v>
+        <f t="shared" si="0"/>
+        <v>0.4385</v>
       </c>
       <c r="G25" s="5">
         <f t="shared" si="1"/>
+        <v>0.51249999999999996</v>
+      </c>
+      <c r="H25" s="5">
+        <f t="shared" si="2"/>
+        <v>0.56930000000000003</v>
+      </c>
+      <c r="I25" s="5">
+        <f t="shared" si="3"/>
+        <v>0.66310000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" t="s">
+        <v>111</v>
+      </c>
+      <c r="D26" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" t="s">
+        <v>35</v>
+      </c>
+      <c r="F26" s="5">
+        <f t="shared" si="0"/>
+        <v>0.38719999999999999</v>
+      </c>
+      <c r="G26" s="5">
+        <f t="shared" si="1"/>
+        <v>0.4572</v>
+      </c>
+      <c r="H26" s="5">
+        <f t="shared" si="2"/>
+        <v>0.51419999999999999</v>
+      </c>
+      <c r="I26" s="5">
+        <f t="shared" si="3"/>
+        <v>0.60680000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" t="s">
+        <v>113</v>
+      </c>
+      <c r="D27" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" t="s">
+        <v>35</v>
+      </c>
+      <c r="F27" s="5">
+        <f t="shared" si="0"/>
+        <v>0.3614</v>
+      </c>
+      <c r="G27" s="5">
+        <f t="shared" si="1"/>
+        <v>0.42770000000000002</v>
+      </c>
+      <c r="H27" s="5">
+        <f t="shared" si="2"/>
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="I27" s="5">
+        <f t="shared" si="3"/>
+        <v>0.57940000000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" t="s">
+        <v>112</v>
+      </c>
+      <c r="D28" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" t="s">
+        <v>35</v>
+      </c>
+      <c r="F28" s="5">
+        <f t="shared" si="0"/>
+        <v>0.35369999999999996</v>
+      </c>
+      <c r="G28" s="5">
+        <f t="shared" si="1"/>
+        <v>0.40429999999999999</v>
+      </c>
+      <c r="H28" s="5">
+        <f t="shared" si="2"/>
+        <v>0.49020000000000002</v>
+      </c>
+      <c r="I28" s="5">
+        <f t="shared" si="3"/>
+        <v>0.56689999999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" t="s">
+        <v>31</v>
+      </c>
+      <c r="F29" s="5">
+        <f t="shared" si="0"/>
+        <v>0.30959999999999999</v>
+      </c>
+      <c r="G29" s="5">
+        <f t="shared" si="1"/>
         <v>0.36380000000000001</v>
       </c>
-      <c r="H25" s="5">
+      <c r="H29" s="5">
+        <f t="shared" si="2"/>
+        <v>0.39490000000000003</v>
+      </c>
+      <c r="I29" s="5">
+        <f t="shared" si="3"/>
+        <v>0.47889999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D30" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" t="s">
+        <v>39</v>
+      </c>
+      <c r="F30" s="5">
+        <f t="shared" si="0"/>
+        <v>0.16969999999999999</v>
+      </c>
+      <c r="G30" s="5">
         <f t="shared" si="1"/>
-        <v>0.47889999999999999</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D29" t="s">
+        <v>0.2009</v>
+      </c>
+      <c r="H30" s="5">
+        <f t="shared" si="2"/>
+        <v>0.29380000000000001</v>
+      </c>
+      <c r="I30" s="5">
+        <f t="shared" si="3"/>
+        <v>0.35249999999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" t="s">
+        <v>114</v>
+      </c>
+      <c r="D31" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" t="s">
+        <v>35</v>
+      </c>
+      <c r="F31" s="5">
+        <f t="shared" si="0"/>
+        <v>0.14419999999999999</v>
+      </c>
+      <c r="G31" s="5">
+        <f t="shared" si="1"/>
+        <v>0.16670000000000001</v>
+      </c>
+      <c r="H31" s="5">
+        <f t="shared" si="2"/>
+        <v>0.27379999999999999</v>
+      </c>
+      <c r="I31" s="5">
+        <f t="shared" si="3"/>
+        <v>0.32329999999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E36" t="s">
         <v>109</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F36" t="s">
         <v>43</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G36" t="s">
+        <v>47</v>
+      </c>
+      <c r="H36" t="s">
         <v>45</v>
       </c>
-      <c r="G29" t="s">
-        <v>47</v>
-      </c>
-      <c r="H29" t="s">
+      <c r="I36" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D30" t="s">
+    <row r="37" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E37" t="s">
         <v>107</v>
       </c>
-      <c r="E30" s="6">
-        <f>E21-E23</f>
-        <v>0.40310000000000001</v>
-      </c>
-      <c r="F30" s="6">
-        <f t="shared" ref="F30:H30" si="2">F21-F23</f>
-        <v>0.35025000000000006</v>
-      </c>
-      <c r="G30" s="6">
-        <f t="shared" si="2"/>
-        <v>0.43965000000000004</v>
-      </c>
-      <c r="H30" s="6">
-        <f t="shared" si="2"/>
-        <v>0.32724999999999993</v>
+      <c r="F37" s="6">
+        <f>F21-F23</f>
+        <v>0.2601</v>
+      </c>
+      <c r="G37" s="6">
+        <f>G21-G23</f>
+        <v>0.30849999999999989</v>
+      </c>
+      <c r="H37" s="6">
+        <f t="shared" ref="G37:I37" si="4">H21-H23</f>
+        <v>0.24649999999999994</v>
+      </c>
+      <c r="I37" s="6">
+        <f t="shared" si="4"/>
+        <v>0.21409999999999996</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H14">
-    <sortCondition descending="1" ref="E2:E14"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I14">
+    <sortCondition descending="1" ref="I2:I14"/>
   </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>